<commit_message>
First pass through 2021 inventories. Found NANOOS inventory from progress report pdf
</commit_message>
<xml_diff>
--- a/2021/data/processed/AOOS.xlsx
+++ b/2021/data/processed/AOOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caroldjanzen/Desktop/ASSET INVENTORY/2021 Asset Inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2021\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DF6D5F2-10A4-BE4D-92C3-2322A6D1DD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F62A977-2A1F-4C8B-BB58-A8FAB04404B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="5480" windowWidth="48440" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="5475" windowWidth="48435" windowHeight="20175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 RA assets" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mathew Biddle</author>
+  </authors>
+  <commentList>
+    <comment ref="G36" authorId="0" shapeId="0" xr:uid="{0C6AC7D1-C623-423A-865F-3F52A1A8BFC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mathew Biddle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+originally -1331.644231</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2485,7 +2519,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2628,6 +2662,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3395,39 +3442,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="23" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="23" customWidth="1"/>
     <col min="4" max="4" width="25" style="23" customWidth="1"/>
-    <col min="5" max="5" width="54.33203125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5" style="25" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="26" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" style="26" customWidth="1"/>
     <col min="12" max="12" width="41" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.83203125" style="23" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="59.83203125" style="23" customWidth="1"/>
-    <col min="17" max="17" width="82.33203125" style="23" customWidth="1"/>
-    <col min="18" max="18" width="90.1640625" style="23" customWidth="1"/>
-    <col min="19" max="19" width="34.1640625" style="23" customWidth="1"/>
-    <col min="20" max="16384" width="9.1640625" style="23"/>
+    <col min="13" max="13" width="43.85546875" style="23" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="59.85546875" style="23" customWidth="1"/>
+    <col min="17" max="17" width="82.28515625" style="23" customWidth="1"/>
+    <col min="18" max="18" width="90.140625" style="23" customWidth="1"/>
+    <col min="19" max="19" width="34.140625" style="23" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="32">
+    <row r="1" spans="1:20" ht="45">
       <c r="A1" s="65" t="s">
         <v>273</v>
       </c>
@@ -3483,7 +3530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="112">
+    <row r="3" spans="1:20" ht="120">
       <c r="A3" s="29" t="s">
         <v>37</v>
       </c>
@@ -3538,7 +3585,7 @@
       </c>
       <c r="S3" s="26"/>
     </row>
-    <row r="4" spans="1:20" ht="96">
+    <row r="4" spans="1:20" ht="105">
       <c r="A4" s="29" t="s">
         <v>37</v>
       </c>
@@ -3592,7 +3639,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="64">
+    <row r="5" spans="1:20" ht="90">
       <c r="A5" s="29" t="s">
         <v>37</v>
       </c>
@@ -3648,7 +3695,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="64">
+    <row r="6" spans="1:20" ht="75">
       <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
@@ -3704,7 +3751,7 @@
       <c r="S6" s="72"/>
       <c r="T6" s="72"/>
     </row>
-    <row r="7" spans="1:20" ht="32">
+    <row r="7" spans="1:20" ht="45">
       <c r="A7" s="48" t="s">
         <v>37</v>
       </c>
@@ -3759,7 +3806,7 @@
       </c>
       <c r="S7" s="74"/>
     </row>
-    <row r="8" spans="1:20" ht="32">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="48" t="s">
         <v>37</v>
       </c>
@@ -3814,7 +3861,7 @@
       </c>
       <c r="S8" s="74"/>
     </row>
-    <row r="9" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="9" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A9" s="75" t="s">
         <v>37</v>
       </c>
@@ -3868,7 +3915,7 @@
       </c>
       <c r="S9" s="77"/>
     </row>
-    <row r="10" spans="1:20" ht="32">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="29" t="s">
         <v>37</v>
       </c>
@@ -3920,7 +3967,7 @@
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
     </row>
-    <row r="11" spans="1:20" ht="32">
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" s="29" t="s">
         <v>37</v>
       </c>
@@ -3975,7 +4022,7 @@
       </c>
       <c r="S11" s="26"/>
     </row>
-    <row r="12" spans="1:20" ht="32">
+    <row r="12" spans="1:20" ht="30">
       <c r="A12" s="29" t="s">
         <v>37</v>
       </c>
@@ -4032,7 +4079,7 @@
       </c>
       <c r="S12" s="26"/>
     </row>
-    <row r="13" spans="1:20" ht="32">
+    <row r="13" spans="1:20" ht="30">
       <c r="A13" s="57" t="s">
         <v>37</v>
       </c>
@@ -4089,7 +4136,7 @@
       </c>
       <c r="S13" s="26"/>
     </row>
-    <row r="14" spans="1:20" s="72" customFormat="1" ht="32">
+    <row r="14" spans="1:20" s="72" customFormat="1" ht="30">
       <c r="A14" s="23" t="s">
         <v>37</v>
       </c>
@@ -4140,7 +4187,7 @@
       </c>
       <c r="R14" s="85"/>
     </row>
-    <row r="15" spans="1:20" ht="16">
+    <row r="15" spans="1:20">
       <c r="A15" s="29" t="s">
         <v>37</v>
       </c>
@@ -4190,7 +4237,7 @@
       <c r="R15" s="26"/>
       <c r="S15" s="87"/>
     </row>
-    <row r="16" spans="1:20" ht="32">
+    <row r="16" spans="1:20" ht="30">
       <c r="A16" s="29" t="s">
         <v>37</v>
       </c>
@@ -4244,7 +4291,7 @@
       </c>
       <c r="S16" s="26"/>
     </row>
-    <row r="17" spans="1:20" ht="32">
+    <row r="17" spans="1:20" ht="30">
       <c r="A17" s="29" t="s">
         <v>37</v>
       </c>
@@ -4296,7 +4343,7 @@
       <c r="S17" s="72"/>
       <c r="T17" s="72"/>
     </row>
-    <row r="18" spans="1:20" ht="32">
+    <row r="18" spans="1:20" ht="30">
       <c r="A18" s="29" t="s">
         <v>37</v>
       </c>
@@ -4352,7 +4399,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="32">
+    <row r="19" spans="1:20" ht="30">
       <c r="A19" s="29" t="s">
         <v>37</v>
       </c>
@@ -4404,7 +4451,7 @@
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
     </row>
-    <row r="20" spans="1:20" ht="32">
+    <row r="20" spans="1:20" ht="30">
       <c r="A20" s="29" t="s">
         <v>37</v>
       </c>
@@ -4460,7 +4507,7 @@
       <c r="S20" s="72"/>
       <c r="T20" s="72"/>
     </row>
-    <row r="21" spans="1:20" ht="32">
+    <row r="21" spans="1:20" ht="30">
       <c r="A21" s="29" t="s">
         <v>37</v>
       </c>
@@ -4513,7 +4560,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="32">
+    <row r="22" spans="1:20" ht="30">
       <c r="A22" s="29" t="s">
         <v>37</v>
       </c>
@@ -4570,7 +4617,7 @@
       </c>
       <c r="S22" s="26"/>
     </row>
-    <row r="23" spans="1:20" ht="32">
+    <row r="23" spans="1:20" ht="30">
       <c r="A23" s="57" t="s">
         <v>37</v>
       </c>
@@ -4627,7 +4674,7 @@
       </c>
       <c r="S23" s="26"/>
     </row>
-    <row r="24" spans="1:20" ht="32">
+    <row r="24" spans="1:20" ht="30">
       <c r="A24" s="29" t="s">
         <v>37</v>
       </c>
@@ -4682,7 +4729,7 @@
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
     </row>
-    <row r="25" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="25" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A25" s="75" t="s">
         <v>37</v>
       </c>
@@ -4739,7 +4786,7 @@
       </c>
       <c r="S25" s="77"/>
     </row>
-    <row r="26" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="26" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A26" s="75" t="s">
         <v>37</v>
       </c>
@@ -4796,7 +4843,7 @@
       </c>
       <c r="S26" s="77"/>
     </row>
-    <row r="27" spans="1:20" ht="32">
+    <row r="27" spans="1:20" ht="30">
       <c r="A27" s="29" t="s">
         <v>37</v>
       </c>
@@ -4851,7 +4898,7 @@
       <c r="R27" s="26"/>
       <c r="S27" s="26"/>
     </row>
-    <row r="28" spans="1:20" ht="32">
+    <row r="28" spans="1:20" ht="30">
       <c r="A28" s="29" t="s">
         <v>37</v>
       </c>
@@ -4909,7 +4956,7 @@
       <c r="S28" s="72"/>
       <c r="T28" s="72"/>
     </row>
-    <row r="29" spans="1:20" ht="32">
+    <row r="29" spans="1:20" ht="30">
       <c r="A29" s="29" t="s">
         <v>37</v>
       </c>
@@ -4966,7 +5013,7 @@
       </c>
       <c r="S29" s="26"/>
     </row>
-    <row r="30" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="30" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A30" s="75" t="s">
         <v>37</v>
       </c>
@@ -5023,7 +5070,7 @@
       </c>
       <c r="S30" s="71"/>
     </row>
-    <row r="31" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="31" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A31" s="75" t="s">
         <v>37</v>
       </c>
@@ -5077,7 +5124,7 @@
       </c>
       <c r="S31" s="71"/>
     </row>
-    <row r="32" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="32" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A32" s="75" t="s">
         <v>37</v>
       </c>
@@ -5134,7 +5181,7 @@
       </c>
       <c r="S32" s="71"/>
     </row>
-    <row r="33" spans="1:20" s="72" customFormat="1" ht="32">
+    <row r="33" spans="1:20" s="72" customFormat="1" ht="30">
       <c r="A33" s="49" t="s">
         <v>37</v>
       </c>
@@ -5188,7 +5235,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="32">
+    <row r="34" spans="1:20" ht="30">
       <c r="A34" s="29" t="s">
         <v>37</v>
       </c>
@@ -5240,7 +5287,7 @@
       <c r="R34" s="26"/>
       <c r="S34" s="26"/>
     </row>
-    <row r="35" spans="1:20" ht="32">
+    <row r="35" spans="1:20" ht="30">
       <c r="A35" s="29" t="s">
         <v>37</v>
       </c>
@@ -5295,7 +5342,7 @@
       <c r="R35" s="26"/>
       <c r="S35" s="87"/>
     </row>
-    <row r="36" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="36" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A36" s="75" t="s">
         <v>37</v>
       </c>
@@ -5315,7 +5362,7 @@
         <v>55.339500000000001</v>
       </c>
       <c r="G36" s="71">
-        <v>-1331.644231</v>
+        <v>-131.64423099999999</v>
       </c>
       <c r="H36" s="71" t="s">
         <v>77</v>
@@ -5352,7 +5399,7 @@
       </c>
       <c r="S36" s="77"/>
     </row>
-    <row r="37" spans="1:20" ht="32">
+    <row r="37" spans="1:20" ht="30">
       <c r="A37" s="23" t="s">
         <v>37</v>
       </c>
@@ -5404,7 +5451,7 @@
       <c r="R37" s="26"/>
       <c r="S37" s="72"/>
     </row>
-    <row r="38" spans="1:20" ht="32">
+    <row r="38" spans="1:20" ht="30">
       <c r="A38" s="29" t="s">
         <v>37</v>
       </c>
@@ -5459,7 +5506,7 @@
       <c r="R38" s="26"/>
       <c r="S38" s="26"/>
     </row>
-    <row r="39" spans="1:20" ht="32">
+    <row r="39" spans="1:20" ht="30">
       <c r="A39" s="29" t="s">
         <v>37</v>
       </c>
@@ -5516,7 +5563,7 @@
       </c>
       <c r="S39" s="26"/>
     </row>
-    <row r="40" spans="1:20" ht="32">
+    <row r="40" spans="1:20" ht="30">
       <c r="A40" s="29" t="s">
         <v>37</v>
       </c>
@@ -5574,7 +5621,7 @@
       <c r="S40" s="72"/>
       <c r="T40" s="72"/>
     </row>
-    <row r="41" spans="1:20" ht="32">
+    <row r="41" spans="1:20" ht="30">
       <c r="A41" s="29" t="s">
         <v>37</v>
       </c>
@@ -5630,7 +5677,7 @@
       <c r="S41" s="72"/>
       <c r="T41" s="72"/>
     </row>
-    <row r="42" spans="1:20" ht="16">
+    <row r="42" spans="1:20">
       <c r="A42" s="29" t="s">
         <v>37</v>
       </c>
@@ -5680,7 +5727,7 @@
       <c r="R42" s="26"/>
       <c r="S42" s="87"/>
     </row>
-    <row r="43" spans="1:20" ht="32">
+    <row r="43" spans="1:20" ht="30">
       <c r="A43" s="57" t="s">
         <v>37</v>
       </c>
@@ -5737,7 +5784,7 @@
       </c>
       <c r="S43" s="87"/>
     </row>
-    <row r="44" spans="1:20" ht="32">
+    <row r="44" spans="1:20" ht="30">
       <c r="A44" s="29" t="s">
         <v>37</v>
       </c>
@@ -5793,7 +5840,7 @@
       <c r="S44" s="72"/>
       <c r="T44" s="72"/>
     </row>
-    <row r="45" spans="1:20" ht="32">
+    <row r="45" spans="1:20" ht="30">
       <c r="A45" s="29" t="s">
         <v>37</v>
       </c>
@@ -5848,7 +5895,7 @@
       <c r="R45" s="26"/>
       <c r="S45" s="26"/>
     </row>
-    <row r="46" spans="1:20" ht="32">
+    <row r="46" spans="1:20" ht="30">
       <c r="A46" s="29" t="s">
         <v>37</v>
       </c>
@@ -5900,7 +5947,7 @@
       <c r="R46" s="26"/>
       <c r="S46" s="26"/>
     </row>
-    <row r="47" spans="1:20" ht="32">
+    <row r="47" spans="1:20" ht="30">
       <c r="A47" s="29" t="s">
         <v>37</v>
       </c>
@@ -5958,7 +6005,7 @@
       <c r="S47" s="72"/>
       <c r="T47" s="72"/>
     </row>
-    <row r="48" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="48" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A48" s="75" t="s">
         <v>37</v>
       </c>
@@ -6012,7 +6059,7 @@
       </c>
       <c r="S48" s="77"/>
     </row>
-    <row r="49" spans="1:19" s="72" customFormat="1" ht="16">
+    <row r="49" spans="1:19" s="72" customFormat="1" ht="30">
       <c r="A49" s="23" t="s">
         <v>37</v>
       </c>
@@ -6068,7 +6115,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="50" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="50" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A50" s="75" t="s">
         <v>37</v>
       </c>
@@ -6125,7 +6172,7 @@
       </c>
       <c r="S50" s="77"/>
     </row>
-    <row r="51" spans="1:19" ht="32">
+    <row r="51" spans="1:19" ht="30">
       <c r="A51" s="29" t="s">
         <v>37</v>
       </c>
@@ -6182,7 +6229,7 @@
       </c>
       <c r="S51" s="26"/>
     </row>
-    <row r="52" spans="1:19" ht="32">
+    <row r="52" spans="1:19" ht="30">
       <c r="A52" s="29" t="s">
         <v>37</v>
       </c>
@@ -6237,7 +6284,7 @@
       <c r="R52" s="26"/>
       <c r="S52" s="26"/>
     </row>
-    <row r="53" spans="1:19" ht="32">
+    <row r="53" spans="1:19" ht="45">
       <c r="A53" s="29" t="s">
         <v>37</v>
       </c>
@@ -6291,7 +6338,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:19" s="59" customFormat="1" ht="32">
+    <row r="54" spans="1:19" s="59" customFormat="1" ht="30">
       <c r="A54" s="57" t="s">
         <v>37</v>
       </c>
@@ -6347,7 +6394,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="32">
+    <row r="55" spans="1:19" ht="30">
       <c r="A55" s="23" t="s">
         <v>37</v>
       </c>
@@ -6402,7 +6449,7 @@
       <c r="R55" s="26"/>
       <c r="S55" s="26"/>
     </row>
-    <row r="56" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="56" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A56" s="75" t="s">
         <v>37</v>
       </c>
@@ -6456,7 +6503,7 @@
       </c>
       <c r="S56" s="77"/>
     </row>
-    <row r="57" spans="1:19" ht="32">
+    <row r="57" spans="1:19" ht="30">
       <c r="A57" s="29" t="s">
         <v>37</v>
       </c>
@@ -6510,7 +6557,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="58" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A58" s="75" t="s">
         <v>37</v>
       </c>
@@ -6567,7 +6614,7 @@
       </c>
       <c r="S58" s="77"/>
     </row>
-    <row r="59" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="59" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A59" s="75" t="s">
         <v>37</v>
       </c>
@@ -6624,7 +6671,7 @@
       </c>
       <c r="S59" s="77"/>
     </row>
-    <row r="60" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="60" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A60" s="75" t="s">
         <v>37</v>
       </c>
@@ -6681,7 +6728,7 @@
       </c>
       <c r="S60" s="77"/>
     </row>
-    <row r="61" spans="1:19" ht="32">
+    <row r="61" spans="1:19" ht="30">
       <c r="A61" s="23" t="s">
         <v>37</v>
       </c>
@@ -6738,7 +6785,7 @@
       </c>
       <c r="S61" s="26"/>
     </row>
-    <row r="62" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="62" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A62" s="75" t="s">
         <v>37</v>
       </c>
@@ -6793,7 +6840,7 @@
       </c>
       <c r="S62" s="77"/>
     </row>
-    <row r="63" spans="1:19" ht="32">
+    <row r="63" spans="1:19" ht="30">
       <c r="A63" s="29" t="s">
         <v>37</v>
       </c>
@@ -6845,7 +6892,7 @@
       <c r="R63" s="26"/>
       <c r="S63" s="26"/>
     </row>
-    <row r="64" spans="1:19" ht="16">
+    <row r="64" spans="1:19">
       <c r="A64" s="29" t="s">
         <v>37</v>
       </c>
@@ -6895,7 +6942,7 @@
       <c r="R64" s="26"/>
       <c r="S64" s="87"/>
     </row>
-    <row r="65" spans="1:20" s="72" customFormat="1" ht="32">
+    <row r="65" spans="1:20" s="72" customFormat="1" ht="30">
       <c r="A65" s="23" t="s">
         <v>37</v>
       </c>
@@ -6946,7 +6993,7 @@
       </c>
       <c r="R65" s="85"/>
     </row>
-    <row r="66" spans="1:20" s="104" customFormat="1" ht="32">
+    <row r="66" spans="1:20" s="104" customFormat="1" ht="30">
       <c r="A66" s="104" t="s">
         <v>37</v>
       </c>
@@ -7000,7 +7047,7 @@
       </c>
       <c r="S66" s="106"/>
     </row>
-    <row r="67" spans="1:20" ht="32">
+    <row r="67" spans="1:20" ht="30">
       <c r="A67" s="57" t="s">
         <v>37</v>
       </c>
@@ -7057,7 +7104,7 @@
       </c>
       <c r="S67" s="72"/>
     </row>
-    <row r="68" spans="1:20" s="75" customFormat="1" ht="32">
+    <row r="68" spans="1:20" s="75" customFormat="1" ht="30">
       <c r="A68" s="75" t="s">
         <v>37</v>
       </c>
@@ -7109,7 +7156,7 @@
       <c r="R68" s="71"/>
       <c r="S68" s="77"/>
     </row>
-    <row r="69" spans="1:20" s="39" customFormat="1" ht="32">
+    <row r="69" spans="1:20" s="39" customFormat="1" ht="45">
       <c r="A69" s="29" t="s">
         <v>37</v>
       </c>
@@ -7166,7 +7213,7 @@
       </c>
       <c r="T69" s="23"/>
     </row>
-    <row r="70" spans="1:20" ht="80">
+    <row r="70" spans="1:20" ht="90">
       <c r="A70" s="29" t="s">
         <v>55</v>
       </c>
@@ -7280,7 +7327,7 @@
       <c r="S71" s="72"/>
       <c r="T71" s="23"/>
     </row>
-    <row r="72" spans="1:20" ht="16">
+    <row r="72" spans="1:20">
       <c r="A72" s="29" t="s">
         <v>37</v>
       </c>
@@ -7334,7 +7381,7 @@
       </c>
       <c r="S72" s="26"/>
     </row>
-    <row r="73" spans="1:20" ht="16">
+    <row r="73" spans="1:20" ht="30">
       <c r="A73" s="29" t="s">
         <v>37</v>
       </c>
@@ -7388,7 +7435,7 @@
       </c>
       <c r="S73" s="26"/>
     </row>
-    <row r="74" spans="1:20" ht="16">
+    <row r="74" spans="1:20" ht="30">
       <c r="A74" s="29" t="s">
         <v>37</v>
       </c>
@@ -7442,7 +7489,7 @@
       </c>
       <c r="S74" s="26"/>
     </row>
-    <row r="75" spans="1:20" ht="32">
+    <row r="75" spans="1:20" ht="30">
       <c r="A75" s="29" t="s">
         <v>37</v>
       </c>
@@ -7496,7 +7543,7 @@
       </c>
       <c r="S75" s="26"/>
     </row>
-    <row r="76" spans="1:20" ht="96">
+    <row r="76" spans="1:20" ht="90">
       <c r="A76" s="29" t="s">
         <v>37</v>
       </c>
@@ -7550,7 +7597,7 @@
       </c>
       <c r="S76" s="26"/>
     </row>
-    <row r="77" spans="1:20" ht="48">
+    <row r="77" spans="1:20" ht="45">
       <c r="A77" s="48" t="s">
         <v>37</v>
       </c>
@@ -7605,7 +7652,7 @@
       </c>
       <c r="S77" s="26"/>
     </row>
-    <row r="78" spans="1:20" ht="48">
+    <row r="78" spans="1:20" ht="60">
       <c r="A78" s="23" t="s">
         <v>37</v>
       </c>
@@ -7659,7 +7706,7 @@
       </c>
       <c r="S78" s="72"/>
     </row>
-    <row r="79" spans="1:20" ht="48">
+    <row r="79" spans="1:20" ht="45">
       <c r="A79" s="29" t="s">
         <v>37</v>
       </c>
@@ -7713,7 +7760,7 @@
       </c>
       <c r="S79" s="72"/>
     </row>
-    <row r="80" spans="1:20" ht="64">
+    <row r="80" spans="1:20" ht="75">
       <c r="A80" s="57" t="s">
         <v>37</v>
       </c>
@@ -7770,7 +7817,7 @@
       </c>
       <c r="S80" s="72"/>
     </row>
-    <row r="81" spans="1:20" ht="64">
+    <row r="81" spans="1:20" ht="75">
       <c r="A81" s="57" t="s">
         <v>37</v>
       </c>
@@ -7827,7 +7874,7 @@
       </c>
       <c r="S81" s="72"/>
     </row>
-    <row r="82" spans="1:20" ht="32">
+    <row r="82" spans="1:20" ht="30">
       <c r="A82" s="29" t="s">
         <v>37</v>
       </c>
@@ -7883,7 +7930,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="32">
+    <row r="83" spans="1:20" ht="45">
       <c r="A83" s="57" t="s">
         <v>37</v>
       </c>
@@ -7939,7 +7986,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="32">
+    <row r="84" spans="1:20" ht="30">
       <c r="A84" s="29" t="s">
         <v>37</v>
       </c>
@@ -7993,7 +8040,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="100" customHeight="1">
+    <row r="85" spans="1:20" ht="99.95" customHeight="1">
       <c r="A85" s="29" t="s">
         <v>37</v>
       </c>
@@ -8048,7 +8095,7 @@
       </c>
       <c r="S85" s="29"/>
     </row>
-    <row r="86" spans="1:20" ht="32">
+    <row r="86" spans="1:20" ht="30">
       <c r="A86" s="48" t="s">
         <v>37</v>
       </c>
@@ -8106,7 +8153,7 @@
       <c r="S86" s="39"/>
       <c r="T86" s="39"/>
     </row>
-    <row r="87" spans="1:20" ht="16">
+    <row r="87" spans="1:20" ht="30">
       <c r="A87" s="121" t="s">
         <v>37</v>
       </c>
@@ -8162,7 +8209,7 @@
       <c r="S87" s="55"/>
       <c r="T87" s="39"/>
     </row>
-    <row r="88" spans="1:20" ht="80">
+    <row r="88" spans="1:20" ht="90">
       <c r="A88" s="29" t="s">
         <v>37</v>
       </c>
@@ -8218,7 +8265,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="16">
+    <row r="89" spans="1:20">
       <c r="A89" s="55" t="s">
         <v>37</v>
       </c>
@@ -8274,7 +8321,7 @@
       <c r="S89" s="55"/>
       <c r="T89" s="39"/>
     </row>
-    <row r="90" spans="1:20" ht="96">
+    <row r="90" spans="1:20" ht="105">
       <c r="A90" s="29" t="s">
         <v>37</v>
       </c>
@@ -8332,7 +8379,7 @@
       <c r="S90" s="39"/>
       <c r="T90" s="39"/>
     </row>
-    <row r="91" spans="1:20" ht="32">
+    <row r="91" spans="1:20" ht="45">
       <c r="A91" s="29" t="s">
         <v>37</v>
       </c>
@@ -8387,7 +8434,7 @@
       </c>
       <c r="S91" s="26"/>
     </row>
-    <row r="92" spans="1:20" ht="48">
+    <row r="92" spans="1:20" ht="45">
       <c r="A92" s="29" t="s">
         <v>37</v>
       </c>
@@ -8442,7 +8489,7 @@
       </c>
       <c r="S92" s="26"/>
     </row>
-    <row r="93" spans="1:20" ht="32">
+    <row r="93" spans="1:20" ht="30">
       <c r="A93" s="29" t="s">
         <v>37</v>
       </c>
@@ -8497,7 +8544,7 @@
       </c>
       <c r="S93" s="26"/>
     </row>
-    <row r="94" spans="1:20" ht="32">
+    <row r="94" spans="1:20" ht="30">
       <c r="A94" s="29" t="s">
         <v>37</v>
       </c>
@@ -8552,7 +8599,7 @@
       </c>
       <c r="S94" s="26"/>
     </row>
-    <row r="95" spans="1:20" ht="32">
+    <row r="95" spans="1:20" ht="30">
       <c r="A95" s="29" t="s">
         <v>37</v>
       </c>
@@ -8607,7 +8654,7 @@
       </c>
       <c r="S95" s="26"/>
     </row>
-    <row r="96" spans="1:20" ht="32">
+    <row r="96" spans="1:20" ht="30">
       <c r="A96" s="29" t="s">
         <v>37</v>
       </c>
@@ -8662,7 +8709,7 @@
       </c>
       <c r="S96" s="26"/>
     </row>
-    <row r="97" spans="1:19" ht="32">
+    <row r="97" spans="1:19" ht="30">
       <c r="A97" s="29" t="s">
         <v>37</v>
       </c>
@@ -8717,7 +8764,7 @@
       </c>
       <c r="S97" s="28"/>
     </row>
-    <row r="98" spans="1:19" ht="32">
+    <row r="98" spans="1:19" ht="45">
       <c r="A98" s="29" t="s">
         <v>37</v>
       </c>
@@ -8772,7 +8819,7 @@
       </c>
       <c r="S98" s="26"/>
     </row>
-    <row r="99" spans="1:19" ht="96">
+    <row r="99" spans="1:19" ht="105">
       <c r="A99" s="29" t="s">
         <v>37</v>
       </c>
@@ -8827,7 +8874,7 @@
       </c>
       <c r="S99" s="26"/>
     </row>
-    <row r="100" spans="1:19" ht="48">
+    <row r="100" spans="1:19" ht="60">
       <c r="A100" s="29" t="s">
         <v>37</v>
       </c>
@@ -8882,7 +8929,7 @@
       </c>
       <c r="S100" s="26"/>
     </row>
-    <row r="101" spans="1:19" ht="48">
+    <row r="101" spans="1:19" ht="45">
       <c r="A101" s="29" t="s">
         <v>37</v>
       </c>
@@ -8937,7 +8984,7 @@
       </c>
       <c r="S101" s="26"/>
     </row>
-    <row r="102" spans="1:19" ht="32">
+    <row r="102" spans="1:19" ht="30">
       <c r="A102" s="48" t="s">
         <v>37</v>
       </c>
@@ -8991,7 +9038,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="48">
+    <row r="103" spans="1:19" ht="75">
       <c r="A103" s="48" t="s">
         <v>37</v>
       </c>
@@ -9045,7 +9092,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="48">
+    <row r="104" spans="1:19" ht="75">
       <c r="A104" s="48" t="s">
         <v>37</v>
       </c>
@@ -9099,7 +9146,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="48">
+    <row r="105" spans="1:19" ht="45">
       <c r="A105" s="29" t="s">
         <v>37</v>
       </c>
@@ -9152,7 +9199,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="96">
+    <row r="106" spans="1:19" ht="120">
       <c r="A106" s="29" t="s">
         <v>37</v>
       </c>
@@ -9205,7 +9252,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="96">
+    <row r="107" spans="1:19" ht="120">
       <c r="A107" s="29" t="s">
         <v>37</v>
       </c>
@@ -9258,7 +9305,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="80">
+    <row r="108" spans="1:19" ht="90">
       <c r="A108" s="59" t="s">
         <v>37</v>
       </c>
@@ -9314,7 +9361,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="80">
+    <row r="109" spans="1:19" ht="90">
       <c r="A109" s="59" t="s">
         <v>37</v>
       </c>
@@ -9370,7 +9417,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="80">
+    <row r="110" spans="1:19" ht="90">
       <c r="A110" s="59" t="s">
         <v>37</v>
       </c>
@@ -9426,7 +9473,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="80">
+    <row r="111" spans="1:19" ht="90">
       <c r="A111" s="59" t="s">
         <v>37</v>
       </c>
@@ -9482,7 +9529,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="80">
+    <row r="112" spans="1:19" ht="75">
       <c r="A112" s="59" t="s">
         <v>37</v>
       </c>
@@ -9538,7 +9585,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="80">
+    <row r="113" spans="1:18" ht="90">
       <c r="A113" s="59" t="s">
         <v>37</v>
       </c>
@@ -9600,7 +9647,7 @@
       <c r="D114" s="29"/>
       <c r="Q114" s="92"/>
     </row>
-    <row r="115" spans="1:18" ht="16">
+    <row r="115" spans="1:18">
       <c r="A115" s="65" t="s">
         <v>623</v>
       </c>
@@ -9608,19 +9655,19 @@
       <c r="C115" s="29"/>
       <c r="D115" s="29"/>
     </row>
-    <row r="116" spans="1:18" ht="32">
+    <row r="116" spans="1:18" ht="45">
       <c r="A116" s="59"/>
       <c r="B116" s="29" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="96">
+    <row r="117" spans="1:18" ht="90">
       <c r="A117" s="112"/>
       <c r="B117" s="29" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="192">
+    <row r="119" spans="1:18" ht="210">
       <c r="A119" s="113" t="s">
         <v>624</v>
       </c>
@@ -9631,6 +9678,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9642,9 +9690,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="208">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="210">
       <c r="A1" s="11" t="s">
         <v>273</v>
       </c>
@@ -9700,7 +9748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="23" customFormat="1" ht="32">
+    <row r="2" spans="1:20" s="23" customFormat="1" ht="255">
       <c r="A2" s="29" t="s">
         <v>37</v>
       </c>
@@ -9754,7 +9802,7 @@
       </c>
       <c r="S2" s="74"/>
     </row>
-    <row r="3" spans="1:20" s="23" customFormat="1" ht="32">
+    <row r="3" spans="1:20" s="23" customFormat="1" ht="255">
       <c r="A3" s="29" t="s">
         <v>37</v>
       </c>
@@ -9808,7 +9856,7 @@
       </c>
       <c r="S3" s="74"/>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" ht="240">
+    <row r="4" spans="1:20" s="5" customFormat="1" ht="270">
       <c r="A4" s="10" t="s">
         <v>37</v>
       </c>
@@ -9862,7 +9910,7 @@
       </c>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" ht="240">
+    <row r="5" spans="1:20" s="5" customFormat="1" ht="270">
       <c r="A5" s="10" t="s">
         <v>37</v>
       </c>
@@ -9916,7 +9964,7 @@
       </c>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" ht="240">
+    <row r="6" spans="1:20" s="5" customFormat="1" ht="270">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -9970,7 +10018,7 @@
       </c>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="240">
+    <row r="7" spans="1:20" s="3" customFormat="1" ht="270">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -10023,7 +10071,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" ht="256">
+    <row r="8" spans="1:20" s="5" customFormat="1" ht="270">
       <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
@@ -10082,7 +10130,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="23" customFormat="1" ht="395">
+    <row r="11" spans="1:20" s="23" customFormat="1" ht="390">
       <c r="A11" s="29" t="s">
         <v>37</v>
       </c>
@@ -10141,7 +10189,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="23" customFormat="1" ht="304">
+    <row r="12" spans="1:20" s="23" customFormat="1" ht="315">
       <c r="A12" s="23" t="s">
         <v>37</v>
       </c>
@@ -10195,7 +10243,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="23" customFormat="1" ht="48">
+    <row r="13" spans="1:20" s="23" customFormat="1" ht="315">
       <c r="A13" s="29" t="s">
         <v>37</v>
       </c>
@@ -10249,7 +10297,7 @@
       </c>
       <c r="S13" s="26"/>
     </row>
-    <row r="15" spans="1:20" ht="160">
+    <row r="15" spans="1:20" ht="165">
       <c r="A15" s="29" t="s">
         <v>37</v>
       </c>
@@ -10368,7 +10416,7 @@
       </c>
       <c r="T16" s="5"/>
     </row>
-    <row r="17" spans="1:19" ht="380">
+    <row r="17" spans="1:19" ht="409.5">
       <c r="A17" s="29" t="s">
         <v>37</v>
       </c>
@@ -10427,7 +10475,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="380">
+    <row r="18" spans="1:19" ht="409.5">
       <c r="A18" s="29" t="s">
         <v>37</v>
       </c>
@@ -10507,7 +10555,7 @@
       <c r="R19" s="41"/>
       <c r="S19" s="126"/>
     </row>
-    <row r="20" spans="1:19" ht="256">
+    <row r="20" spans="1:19" ht="270">
       <c r="A20" s="29" t="s">
         <v>37</v>
       </c>
@@ -10579,28 +10627,28 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="46.33203125" customWidth="1"/>
-    <col min="18" max="18" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="46.28515625" customWidth="1"/>
+    <col min="18" max="18" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="64">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="60">
       <c r="A1" s="11" t="s">
         <v>273</v>
       </c>
@@ -10656,7 +10704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="18" customFormat="1" ht="80">
+    <row r="2" spans="1:20" s="18" customFormat="1" ht="120">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
@@ -10712,7 +10760,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:20" s="37" customFormat="1" ht="96">
+    <row r="3" spans="1:20" s="37" customFormat="1" ht="105">
       <c r="A3" s="33" t="s">
         <v>37</v>
       </c>
@@ -10768,7 +10816,7 @@
       <c r="S3" s="34"/>
       <c r="T3" s="38"/>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="96">
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A4" s="10" t="s">
         <v>37</v>
       </c>
@@ -10818,7 +10866,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="80">
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A5" s="10" t="s">
         <v>37</v>
       </c>
@@ -10868,7 +10916,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="41" customFormat="1" ht="80">
+    <row r="7" spans="1:20" s="41" customFormat="1" ht="90">
       <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
@@ -10917,7 +10965,7 @@
     </row>
     <row r="8" spans="1:20" s="41" customFormat="1"/>
     <row r="9" spans="1:20" s="41" customFormat="1"/>
-    <row r="10" spans="1:20" s="41" customFormat="1" ht="272">
+    <row r="10" spans="1:20" s="41" customFormat="1" ht="270">
       <c r="A10" s="41" t="s">
         <v>37</v>
       </c>
@@ -10983,15 +11031,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="139"/>
-    <col min="4" max="4" width="26.83203125" style="139" customWidth="1"/>
-    <col min="5" max="18" width="10.83203125" style="139"/>
-    <col min="19" max="16384" width="10.83203125" style="135"/>
+    <col min="1" max="3" width="10.85546875" style="139"/>
+    <col min="4" max="4" width="26.85546875" style="139" customWidth="1"/>
+    <col min="5" max="18" width="10.85546875" style="139"/>
+    <col min="19" max="16384" width="10.85546875" style="135"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="23" customFormat="1" ht="208">
+    <row r="1" spans="1:19" s="23" customFormat="1" ht="240">
       <c r="A1" s="65" t="s">
         <v>273</v>
       </c>
@@ -11047,7 +11095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="72" customFormat="1" ht="32">
+    <row r="3" spans="1:19" s="72" customFormat="1" ht="30">
       <c r="A3" s="57" t="s">
         <v>37</v>
       </c>
@@ -11089,7 +11137,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="72" customFormat="1" ht="32">
+    <row r="4" spans="1:19" s="72" customFormat="1" ht="30">
       <c r="A4" s="59" t="s">
         <v>37</v>
       </c>
@@ -11131,7 +11179,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="75" customFormat="1" ht="32">
+    <row r="5" spans="1:19" s="75" customFormat="1" ht="30">
       <c r="A5" s="59" t="s">
         <v>37</v>
       </c>
@@ -11174,7 +11222,7 @@
       </c>
       <c r="S5" s="77"/>
     </row>
-    <row r="6" spans="1:19" s="54" customFormat="1" ht="32">
+    <row r="6" spans="1:19" s="54" customFormat="1" ht="30">
       <c r="A6" s="59" t="s">
         <v>37</v>
       </c>
@@ -11216,7 +11264,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="54" customFormat="1" ht="32">
+    <row r="7" spans="1:19" s="54" customFormat="1" ht="30">
       <c r="A7" s="59" t="s">
         <v>37</v>
       </c>
@@ -11258,7 +11306,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="54" customFormat="1" ht="32">
+    <row r="8" spans="1:19" s="54" customFormat="1" ht="30">
       <c r="A8" s="59" t="s">
         <v>37</v>
       </c>
@@ -11300,7 +11348,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="54" customFormat="1" ht="144">
+    <row r="9" spans="1:19" s="54" customFormat="1" ht="135">
       <c r="A9" s="59" t="s">
         <v>55</v>
       </c>
@@ -11342,7 +11390,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="54" customFormat="1" ht="64">
+    <row r="10" spans="1:19" s="54" customFormat="1" ht="60">
       <c r="A10" s="59" t="s">
         <v>37</v>
       </c>
@@ -11384,7 +11432,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="256">
+    <row r="11" spans="1:19" ht="255">
       <c r="A11" s="137" t="s">
         <v>37</v>
       </c>
@@ -11426,7 +11474,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="176">
+    <row r="12" spans="1:19" ht="195">
       <c r="A12" s="137" t="s">
         <v>37</v>
       </c>
@@ -11468,7 +11516,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="224">
+    <row r="13" spans="1:19" ht="240">
       <c r="A13" s="139" t="s">
         <v>37</v>
       </c>
@@ -11492,19 +11540,19 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="59.33203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="59.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="17" max="17" width="85.33203125" customWidth="1"/>
+    <col min="17" max="17" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="32">
+    <row r="1" spans="1:18" s="5" customFormat="1" ht="30">
       <c r="A1" s="11" t="s">
         <v>273</v>
       </c>
@@ -11560,7 +11608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" ht="160">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="180">
       <c r="A2" s="6" t="s">
         <v>275</v>
       </c>

</xml_diff>